<commit_message>
BREAKING CHANGE feat(emx2) can now choose column names for composite foreign keys
</commit_message>
<xml_diff>
--- a/backend/molgenis-emx2-linkeddata/src/test/resources/fdp.xlsx
+++ b/backend/molgenis-emx2-linkeddata/src/test/resources/fdp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umcg-mswertz/IdeaProjects/emx2/backend/molgenis-emx2-linkeddata/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6767123A-BBD7-0848-B9E3-373A7E96E898}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF27D81D-0B85-5945-A601-11BF455F73D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{FC3106C0-1D46-C24B-9B5F-C0729D326D4C}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="48">
   <si>
     <t>tableName</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>ttlTemplate</t>
+  </si>
+  <si>
+    <t>refTable</t>
   </si>
 </sst>
 </file>
@@ -586,7 +589,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,7 +619,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>33</v>

</xml_diff>